<commit_message>
P4-2214 changes to include the prices used for the calculations to an extra tab in the output spreadsheet.
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/JCP_template.xlsx
+++ b/src/main/resources/spreadsheets/JCP_template.xlsx
@@ -1,27 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonnycavell/p/calculate-people-move-prices/src/main/resources/spreadsheets/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3CE9D3-CCCB-1547-A942-6076D589A345}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29580" windowHeight="17140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Standard" sheetId="2" r:id="rId2"/>
-    <sheet name="Long haul" sheetId="3" r:id="rId3"/>
-    <sheet name="Redirections" sheetId="4" r:id="rId4"/>
-    <sheet name="Lockouts" sheetId="5" r:id="rId5"/>
-    <sheet name="Multi-type" sheetId="6" r:id="rId6"/>
-    <sheet name="JPC_Serco_300120_v8" sheetId="7" r:id="rId7"/>
+    <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Standard" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Long haul" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Redirections" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Lockouts" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Multi-type" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="JPC_Serco_300120_v8" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="JPC Price book" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -33,103 +29,103 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="55">
   <si>
-    <t>Export date</t>
-  </si>
-  <si>
-    <t>Export from previous day's events</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>JPC_Serco_300120_v8</t>
-  </si>
-  <si>
-    <t>Need to agree name of file</t>
-  </si>
-  <si>
-    <t>Calculate Journey Variable Payments (S2B)</t>
-  </si>
-  <si>
-    <t>Dev Notes:</t>
-  </si>
-  <si>
-    <t>Supplier</t>
-  </si>
-  <si>
-    <t>SERCO</t>
-  </si>
-  <si>
-    <t>Date Range</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>All completed moves</t>
-  </si>
-  <si>
-    <t>OUTPUT SUMMARY</t>
-  </si>
-  <si>
-    <t>Move type</t>
-  </si>
-  <si>
-    <t>Percentage</t>
+    <t xml:space="preserve">Export date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Export from previous day's events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JPC_Serco_300120_v8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to agree name of file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate Journey Variable Payments (S2B)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dev Notes:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All completed moves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUTPUT SUMMARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage</t>
   </si>
   <si>
     <t xml:space="preserve"> Volume</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Standard move</t>
-  </si>
-  <si>
-    <t>includes single journeys, cross supplier and redirects before the move has started</t>
-  </si>
-  <si>
-    <t>Standard move without prices</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>move not found in JPC</t>
+    <t xml:space="preserve">Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard move</t>
+  </si>
+  <si>
+    <t xml:space="preserve">includes single journeys, cross supplier and redirects before the move has started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard move without prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--</t>
+  </si>
+  <si>
+    <t xml:space="preserve">move not found in JPC</t>
   </si>
   <si>
     <t xml:space="preserve">Long haul </t>
   </si>
   <si>
-    <t>a completed move made up of 2 or more journeys</t>
-  </si>
-  <si>
-    <t>Redirections</t>
-  </si>
-  <si>
-    <t>a redirection after the move has started</t>
-  </si>
-  <si>
-    <t>Lockouts</t>
-  </si>
-  <si>
-    <t>refused admission to prison</t>
-  </si>
-  <si>
-    <t>Multi-type moves</t>
-  </si>
-  <si>
-    <t>includes combinations of the above</t>
-  </si>
-  <si>
-    <t>Total %</t>
-  </si>
-  <si>
-    <t>Total Volume</t>
-  </si>
-  <si>
-    <t>Total Price</t>
+    <t xml:space="preserve">a completed move made up of 2 or more journeys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redirections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a redirection after the move has started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lockouts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refused admission to prison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-type moves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">includes combinations of the above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Price</t>
   </si>
   <si>
     <r>
@@ -137,64 +133,66 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">STANDARD MOVES </t>
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="11"/>
         <rFont val="Cambria"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t>(includes single journeys, cross supplier and redirects before the move has started)</t>
+      <t xml:space="preserve">(includes single journeys, cross supplier and redirects before the move has started)</t>
     </r>
   </si>
   <si>
-    <t>Move Ref ID</t>
-  </si>
-  <si>
-    <t>Pick up</t>
-  </si>
-  <si>
-    <t>Location Type</t>
-  </si>
-  <si>
-    <t>Drop off</t>
-  </si>
-  <si>
-    <t>Pick up date</t>
-  </si>
-  <si>
-    <t>Pick up time</t>
-  </si>
-  <si>
-    <t>Drop off date</t>
-  </si>
-  <si>
-    <t>Drop off time</t>
-  </si>
-  <si>
-    <t>Vehicle Reg No</t>
-  </si>
-  <si>
-    <t>NOMIS Prison ID</t>
-  </si>
-  <si>
-    <t>LONG HAUL</t>
-  </si>
-  <si>
-    <t>Move ID</t>
-  </si>
-  <si>
-    <t>Vehicle ID</t>
-  </si>
-  <si>
-    <t>Contractor Billable?</t>
-  </si>
-  <si>
-    <t>Notes</t>
+    <t xml:space="preserve">Move Ref ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop off date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop off time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle Reg No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOMIS Prison ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LONG HAUL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contractor Billable?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
   </si>
   <si>
     <r>
@@ -202,27 +200,30 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">REDIRECTIONS </t>
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="11"/>
         <rFont val="Cambria"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t>(a redirection after the move has started)</t>
+      <t xml:space="preserve">(a redirection after the move has started)</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
-        <b/>
+        <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Notes </t>
@@ -231,9 +232,10 @@
       <rPr>
         <sz val="11"/>
         <rFont val="Cambria"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t>(Reason codes or supplier notes)</t>
+      <t xml:space="preserve">(Reason codes or supplier notes)</t>
     </r>
   </si>
   <si>
@@ -242,22 +244,24 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">LOCKOUTS </t>
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="9"/>
         <rFont val="Cambria"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t>(refused admission to prison)</t>
+      <t xml:space="preserve">(refused admission to prison)</t>
     </r>
   </si>
   <si>
-    <t>Date range</t>
+    <t xml:space="preserve">Date range</t>
   </si>
   <si>
     <r>
@@ -265,92 +269,123 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t>MULTI-TYPE MOVES</t>
+      <t xml:space="preserve">MULTI-TYPE MOVES</t>
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="11"/>
         <rFont val="Cambria"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> (includes combinations of move types)</t>
     </r>
   </si>
   <si>
-    <t>This needs to be either password protected or interstitial confidentiality agreement per Commercials req</t>
+    <t xml:space="preserve">This needs to be either password protected or interstitial confidentiality agreement per Commercials req</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="\£#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="6">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="0%"/>
+    <numFmt numFmtId="167" formatCode="#,##0"/>
+    <numFmt numFmtId="168" formatCode="\£#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <i val="true"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <i val="true"/>
       <sz val="11"/>
       <name val="Cambria"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <i val="true"/>
       <sz val="9"/>
       <name val="Cambria"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -411,7 +446,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -419,91 +454,197 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="39">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -562,342 +703,36 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
-    <col min="5" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="2" t="n">
         <v>43862</v>
       </c>
       <c r="C1" s="3"/>
@@ -927,7 +762,7 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" spans="1:26" ht="15">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -960,7 +795,7 @@
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
     </row>
-    <row r="3" spans="1:26" ht="14">
+    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -987,7 +822,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26" ht="14">
+    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -1018,7 +853,7 @@
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
     </row>
-    <row r="5" spans="1:26" ht="14">
+    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1049,17 +884,17 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26" ht="14">
+    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="9" t="n">
         <v>43831</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="9" t="n">
         <v>43861</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -1086,7 +921,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:26" ht="14">
+    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1114,7 +949,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26" ht="14">
+    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
@@ -1144,7 +979,7 @@
       <c r="Y8" s="11"/>
       <c r="Z8" s="11"/>
     </row>
-    <row r="9" spans="1:26" ht="14">
+    <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
@@ -1180,17 +1015,17 @@
       <c r="Y9" s="14"/>
       <c r="Z9" s="14"/>
     </row>
-    <row r="10" spans="1:26" ht="14">
+    <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="16" t="n">
         <v>0.9</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="17" t="n">
         <v>9000</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="18" t="n">
         <v>90000</v>
       </c>
       <c r="E10" s="3"/>
@@ -1216,7 +1051,7 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
     </row>
-    <row r="11" spans="1:26" ht="14">
+    <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
         <v>18</v>
       </c>
@@ -1246,7 +1081,7 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" ht="14">
+    <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="20"/>
@@ -1274,14 +1109,14 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26" ht="14">
+    <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="16" t="n">
         <v>0.05</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="17" t="n">
         <v>500</v>
       </c>
       <c r="D13" s="22" t="s">
@@ -1310,7 +1145,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:26" ht="14">
+    <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="s">
         <v>21</v>
       </c>
@@ -1340,7 +1175,7 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:26" ht="14">
+    <row r="15" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1368,14 +1203,14 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:26" ht="14">
+    <row r="16" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="24" t="n">
         <v>0.01</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="15" t="n">
         <v>100</v>
       </c>
       <c r="D16" s="22" t="s">
@@ -1404,7 +1239,7 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:26" ht="14">
+    <row r="17" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19" t="s">
         <v>23</v>
       </c>
@@ -1431,7 +1266,7 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:26" ht="14">
+    <row r="18" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="19"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1459,14 +1294,14 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
     </row>
-    <row r="19" spans="1:26" ht="14">
+    <row r="19" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="16" t="n">
         <v>0.01</v>
       </c>
-      <c r="C19" s="25">
+      <c r="C19" s="25" t="n">
         <v>100</v>
       </c>
       <c r="D19" s="22" t="s">
@@ -1495,7 +1330,7 @@
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
     </row>
-    <row r="20" spans="1:26" ht="14">
+    <row r="20" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="19" t="s">
         <v>25</v>
       </c>
@@ -1525,7 +1360,7 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
     </row>
-    <row r="21" spans="1:26" ht="14">
+    <row r="21" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1553,14 +1388,14 @@
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
     </row>
-    <row r="22" spans="1:26" ht="14">
+    <row r="22" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="16">
+      <c r="B22" s="16" t="n">
         <v>0.01</v>
       </c>
-      <c r="C22" s="25">
+      <c r="C22" s="25" t="n">
         <v>100</v>
       </c>
       <c r="D22" s="22" t="s">
@@ -1589,7 +1424,7 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" ht="14">
+    <row r="23" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="19" t="s">
         <v>27</v>
       </c>
@@ -1619,7 +1454,7 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
     </row>
-    <row r="24" spans="1:26" ht="14">
+    <row r="24" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1647,14 +1482,14 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
     </row>
-    <row r="25" spans="1:26" ht="14">
+    <row r="25" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="16">
+      <c r="B25" s="16" t="n">
         <v>0.02</v>
       </c>
-      <c r="C25" s="25">
+      <c r="C25" s="25" t="n">
         <v>200</v>
       </c>
       <c r="D25" s="22" t="s">
@@ -1683,7 +1518,7 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
     </row>
-    <row r="26" spans="1:26" ht="14">
+    <row r="26" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="19" t="s">
         <v>29</v>
       </c>
@@ -1713,7 +1548,7 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
     </row>
-    <row r="27" spans="1:26" ht="14">
+    <row r="27" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1741,7 +1576,7 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
     </row>
-    <row r="28" spans="1:26" ht="14">
+    <row r="28" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8"/>
       <c r="B28" s="26" t="s">
         <v>30</v>
@@ -1775,12 +1610,12 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
     </row>
-    <row r="29" spans="1:26" ht="14">
+    <row r="29" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3"/>
-      <c r="B29" s="27">
+      <c r="B29" s="27" t="n">
         <v>100</v>
       </c>
-      <c r="C29" s="17">
+      <c r="C29" s="17" t="n">
         <v>10000</v>
       </c>
       <c r="D29" s="22" t="s">
@@ -1809,7 +1644,7 @@
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
     </row>
-    <row r="30" spans="1:26" ht="14">
+    <row r="30" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
       <c r="B30" s="24"/>
       <c r="C30" s="3"/>
@@ -1837,7 +1672,7 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
     </row>
-    <row r="31" spans="1:26" ht="14">
+    <row r="31" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1865,36 +1700,44 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="28"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" customWidth="1"/>
-    <col min="11" max="11" width="18.5" customWidth="1"/>
-    <col min="12" max="1022" width="14.5" customWidth="1"/>
-    <col min="1023" max="1025" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="12" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="14">
+    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1928,7 +1771,7 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="2" spans="1:30" ht="14">
+    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1961,7 +1804,7 @@
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
     </row>
-    <row r="3" spans="1:30" ht="14">
+    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1992,7 +1835,7 @@
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
     </row>
-    <row r="4" spans="1:30" ht="14">
+    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -2026,7 +1869,7 @@
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
     </row>
-    <row r="5" spans="1:30" ht="14">
+    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2060,7 +1903,7 @@
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
     </row>
-    <row r="6" spans="1:30" ht="14">
+    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -2096,7 +1939,7 @@
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
     </row>
-    <row r="7" spans="1:30" ht="14">
+    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2128,7 +1971,7 @@
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
     </row>
-    <row r="8" spans="1:30" ht="14">
+    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>33</v>
       </c>
@@ -2162,7 +2005,7 @@
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
     </row>
-    <row r="9" spans="1:30" ht="12.75" customHeight="1">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
         <v>34</v>
       </c>
@@ -2218,73 +2061,81 @@
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
     </row>
-    <row r="1048540" ht="12.75" customHeight="1"/>
-    <row r="1048541" ht="12.75" customHeight="1"/>
-    <row r="1048542" ht="12.75" customHeight="1"/>
-    <row r="1048543" ht="12.75" customHeight="1"/>
-    <row r="1048544" ht="12.75" customHeight="1"/>
-    <row r="1048545" ht="12.75" customHeight="1"/>
-    <row r="1048546" ht="12.75" customHeight="1"/>
-    <row r="1048547" ht="12.75" customHeight="1"/>
-    <row r="1048548" ht="12.75" customHeight="1"/>
-    <row r="1048549" ht="12.75" customHeight="1"/>
-    <row r="1048550" ht="12.75" customHeight="1"/>
-    <row r="1048551" ht="12.75" customHeight="1"/>
-    <row r="1048552" ht="12.75" customHeight="1"/>
-    <row r="1048553" ht="12.75" customHeight="1"/>
-    <row r="1048554" ht="12.75" customHeight="1"/>
-    <row r="1048555" ht="12.75" customHeight="1"/>
-    <row r="1048556" ht="12.75" customHeight="1"/>
-    <row r="1048557" ht="12.75" customHeight="1"/>
-    <row r="1048558" ht="12.75" customHeight="1"/>
-    <row r="1048559" ht="12.75" customHeight="1"/>
-    <row r="1048560" ht="12.75" customHeight="1"/>
-    <row r="1048561" ht="12.75" customHeight="1"/>
-    <row r="1048562" ht="12.75" customHeight="1"/>
-    <row r="1048563" ht="12.75" customHeight="1"/>
-    <row r="1048564" ht="12.75" customHeight="1"/>
-    <row r="1048565" ht="12.75" customHeight="1"/>
-    <row r="1048566" ht="12.75" customHeight="1"/>
-    <row r="1048567" ht="12.75" customHeight="1"/>
-    <row r="1048568" ht="12.75" customHeight="1"/>
-    <row r="1048569" ht="12.75" customHeight="1"/>
-    <row r="1048570" ht="12.75" customHeight="1"/>
-    <row r="1048571" ht="12.75" customHeight="1"/>
-    <row r="1048572" ht="12.75" customHeight="1"/>
-    <row r="1048573" ht="12.75" customHeight="1"/>
-    <row r="1048574" ht="12.75" customHeight="1"/>
-    <row r="1048575" ht="12.75" customHeight="1"/>
-    <row r="1048576" ht="12.75" customHeight="1"/>
+    <row r="1048540" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="48.5" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" customWidth="1"/>
-    <col min="12" max="12" width="14.5" customWidth="1"/>
-    <col min="13" max="13" width="20.5" customWidth="1"/>
-    <col min="14" max="14" width="24.83203125" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="24.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14">
+    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2302,7 +2153,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:26" ht="14">
+    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2319,7 +2170,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:26" ht="14">
+    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2334,7 +2185,7 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:26" ht="14">
+    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -2352,7 +2203,7 @@
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
     </row>
-    <row r="5" spans="1:26" ht="14">
+    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2370,7 +2221,7 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:26" ht="14">
+    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -2390,7 +2241,7 @@
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:26" ht="14">
+    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2406,7 +2257,7 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:26" ht="14">
+    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
@@ -2424,7 +2275,7 @@
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
     </row>
-    <row r="9" spans="1:26" ht="30">
+    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
         <v>45</v>
       </c>
@@ -2480,39 +2331,47 @@
       <c r="Y9" s="34"/>
       <c r="Z9" s="34"/>
     </row>
-    <row r="1048561" ht="15.75" customHeight="1"/>
-    <row r="1048562" ht="12.75" customHeight="1"/>
-    <row r="1048576" ht="12.75" customHeight="1"/>
+    <row r="1048561" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD1048576"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="52" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="18.5" customWidth="1"/>
-    <col min="12" max="12" width="9.1640625" customWidth="1"/>
-    <col min="13" max="13" width="20.1640625" customWidth="1"/>
-    <col min="14" max="14" width="32.5" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="32.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="14">
+    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2546,7 +2405,7 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="2" spans="1:30" ht="14">
+    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2579,7 +2438,7 @@
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
     </row>
-    <row r="3" spans="1:30" ht="14">
+    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2610,7 +2469,7 @@
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
     </row>
-    <row r="4" spans="1:30" ht="14">
+    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -2644,7 +2503,7 @@
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
     </row>
-    <row r="5" spans="1:30" ht="14">
+    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2678,7 +2537,7 @@
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
     </row>
-    <row r="6" spans="1:30" ht="14">
+    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -2714,7 +2573,7 @@
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
     </row>
-    <row r="7" spans="1:30" ht="14">
+    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2746,7 +2605,7 @@
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
     </row>
-    <row r="8" spans="1:30" ht="14">
+    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>49</v>
       </c>
@@ -2780,7 +2639,7 @@
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
     </row>
-    <row r="9" spans="1:30" ht="45">
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
         <v>45</v>
       </c>
@@ -2840,48 +2699,56 @@
       <c r="AC9" s="15"/>
       <c r="AD9" s="15"/>
     </row>
-    <row r="1048562" ht="12.75" customHeight="1"/>
-    <row r="1048563" ht="12.75" customHeight="1"/>
-    <row r="1048564" ht="12.75" customHeight="1"/>
-    <row r="1048565" ht="12.75" customHeight="1"/>
-    <row r="1048566" ht="12.75" customHeight="1"/>
-    <row r="1048567" ht="12.75" customHeight="1"/>
-    <row r="1048568" ht="12.75" customHeight="1"/>
-    <row r="1048569" ht="12.75" customHeight="1"/>
-    <row r="1048570" ht="12.75" customHeight="1"/>
-    <row r="1048571" ht="12.75" customHeight="1"/>
-    <row r="1048572" ht="12.75" customHeight="1"/>
-    <row r="1048573" ht="12.75" customHeight="1"/>
-    <row r="1048574" ht="12.75" customHeight="1"/>
-    <row r="1048575" ht="12.75" customHeight="1"/>
-    <row r="1048576" ht="12.75" customHeight="1"/>
+    <row r="1048562" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AF1048576"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="7.1640625" customWidth="1"/>
-    <col min="4" max="4" width="28.5" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" customWidth="1"/>
-    <col min="6" max="13" width="14.5" customWidth="1"/>
-    <col min="14" max="14" width="31.33203125" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="31.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="14">
+    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2917,7 +2784,7 @@
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
     </row>
-    <row r="2" spans="1:32" ht="14">
+    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2952,7 +2819,7 @@
       <c r="AE2" s="3"/>
       <c r="AF2" s="3"/>
     </row>
-    <row r="3" spans="1:32" ht="14">
+    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2985,7 +2852,7 @@
       <c r="AE3" s="3"/>
       <c r="AF3" s="3"/>
     </row>
-    <row r="4" spans="1:32" ht="14">
+    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -3021,7 +2888,7 @@
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
     </row>
-    <row r="5" spans="1:32" ht="14">
+    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -3057,7 +2924,7 @@
       <c r="AE5" s="3"/>
       <c r="AF5" s="3"/>
     </row>
-    <row r="6" spans="1:32" ht="14">
+    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -3095,7 +2962,7 @@
       <c r="AE6" s="3"/>
       <c r="AF6" s="3"/>
     </row>
-    <row r="7" spans="1:32" ht="14">
+    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -3129,7 +2996,7 @@
       <c r="AE7" s="3"/>
       <c r="AF7" s="3"/>
     </row>
-    <row r="8" spans="1:32" ht="14">
+    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>51</v>
       </c>
@@ -3165,7 +3032,7 @@
       <c r="AE8" s="3"/>
       <c r="AF8" s="3"/>
     </row>
-    <row r="9" spans="1:32" ht="45">
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
         <v>34</v>
       </c>
@@ -3227,57 +3094,65 @@
       <c r="AE9" s="3"/>
       <c r="AF9" s="3"/>
     </row>
-    <row r="1048559" ht="12.75" customHeight="1"/>
-    <row r="1048560" ht="12.75" customHeight="1"/>
-    <row r="1048561" ht="12.75" customHeight="1"/>
-    <row r="1048562" ht="12.75" customHeight="1"/>
-    <row r="1048563" ht="12.75" customHeight="1"/>
-    <row r="1048564" ht="12.75" customHeight="1"/>
-    <row r="1048565" ht="12.75" customHeight="1"/>
-    <row r="1048566" ht="12.75" customHeight="1"/>
-    <row r="1048567" ht="12.75" customHeight="1"/>
-    <row r="1048568" ht="12.75" customHeight="1"/>
-    <row r="1048569" ht="12.75" customHeight="1"/>
-    <row r="1048570" ht="12.75" customHeight="1"/>
-    <row r="1048571" ht="12.75" customHeight="1"/>
-    <row r="1048572" ht="12.75" customHeight="1"/>
-    <row r="1048573" ht="12.75" customHeight="1"/>
-    <row r="1048574" ht="12.75" customHeight="1"/>
-    <row r="1048575" ht="12.75" customHeight="1"/>
-    <row r="1048576" ht="12.75" customHeight="1"/>
+    <row r="1048559" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L24" activeCellId="0" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="66.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.1640625" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.5" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" customWidth="1"/>
-    <col min="9" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" customWidth="1"/>
-    <col min="13" max="13" width="10.1640625" customWidth="1"/>
-    <col min="14" max="14" width="30" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="30.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="14">
+    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3311,7 +3186,7 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="2" spans="1:30" ht="14">
+    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3344,7 +3219,7 @@
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
     </row>
-    <row r="3" spans="1:30" ht="14">
+    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -3375,7 +3250,7 @@
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
     </row>
-    <row r="4" spans="1:30" ht="14">
+    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -3409,7 +3284,7 @@
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
     </row>
-    <row r="5" spans="1:30" ht="14">
+    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -3443,7 +3318,7 @@
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
     </row>
-    <row r="6" spans="1:30" ht="14">
+    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -3479,7 +3354,7 @@
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
     </row>
-    <row r="7" spans="1:30" ht="14">
+    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -3511,7 +3386,7 @@
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
     </row>
-    <row r="8" spans="1:30" ht="14">
+    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>53</v>
       </c>
@@ -3545,7 +3420,7 @@
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
     </row>
-    <row r="9" spans="1:30" ht="30">
+    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
         <v>45</v>
       </c>
@@ -3605,49 +3480,90 @@
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
     </row>
-    <row r="1048559" ht="12.75" customHeight="1"/>
-    <row r="1048560" ht="12.75" customHeight="1"/>
-    <row r="1048561" ht="12.75" customHeight="1"/>
-    <row r="1048562" ht="12.75" customHeight="1"/>
-    <row r="1048563" ht="12.75" customHeight="1"/>
-    <row r="1048564" ht="12.75" customHeight="1"/>
-    <row r="1048565" ht="12.75" customHeight="1"/>
-    <row r="1048566" ht="12.75" customHeight="1"/>
-    <row r="1048567" ht="12.75" customHeight="1"/>
-    <row r="1048568" ht="12.75" customHeight="1"/>
-    <row r="1048569" ht="12.75" customHeight="1"/>
-    <row r="1048570" ht="12.75" customHeight="1"/>
-    <row r="1048571" ht="12.75" customHeight="1"/>
-    <row r="1048572" ht="12.75" customHeight="1"/>
-    <row r="1048573" ht="12.75" customHeight="1"/>
-    <row r="1048574" ht="12.75" customHeight="1"/>
-    <row r="1048575" ht="12.75" customHeight="1"/>
-    <row r="1048576" ht="12.75" customHeight="1"/>
+    <row r="1048559" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="43" customWidth="1"/>
-    <col min="2" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="45">
+    <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
P4-2214 changes to include the prices used for the calculations to an extra tab in the output spreadsheet. (#49)
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/JCP_template.xlsx
+++ b/src/main/resources/spreadsheets/JCP_template.xlsx
@@ -1,27 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonnycavell/p/calculate-people-move-prices/src/main/resources/spreadsheets/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3CE9D3-CCCB-1547-A942-6076D589A345}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29580" windowHeight="17140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Standard" sheetId="2" r:id="rId2"/>
-    <sheet name="Long haul" sheetId="3" r:id="rId3"/>
-    <sheet name="Redirections" sheetId="4" r:id="rId4"/>
-    <sheet name="Lockouts" sheetId="5" r:id="rId5"/>
-    <sheet name="Multi-type" sheetId="6" r:id="rId6"/>
-    <sheet name="JPC_Serco_300120_v8" sheetId="7" r:id="rId7"/>
+    <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Standard" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Long haul" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Redirections" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Lockouts" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Multi-type" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="JPC_Serco_300120_v8" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="JPC Price book" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -33,103 +29,103 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="55">
   <si>
-    <t>Export date</t>
-  </si>
-  <si>
-    <t>Export from previous day's events</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>JPC_Serco_300120_v8</t>
-  </si>
-  <si>
-    <t>Need to agree name of file</t>
-  </si>
-  <si>
-    <t>Calculate Journey Variable Payments (S2B)</t>
-  </si>
-  <si>
-    <t>Dev Notes:</t>
-  </si>
-  <si>
-    <t>Supplier</t>
-  </si>
-  <si>
-    <t>SERCO</t>
-  </si>
-  <si>
-    <t>Date Range</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>All completed moves</t>
-  </si>
-  <si>
-    <t>OUTPUT SUMMARY</t>
-  </si>
-  <si>
-    <t>Move type</t>
-  </si>
-  <si>
-    <t>Percentage</t>
+    <t xml:space="preserve">Export date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Export from previous day's events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JPC_Serco_300120_v8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to agree name of file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate Journey Variable Payments (S2B)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dev Notes:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All completed moves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUTPUT SUMMARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage</t>
   </si>
   <si>
     <t xml:space="preserve"> Volume</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Standard move</t>
-  </si>
-  <si>
-    <t>includes single journeys, cross supplier and redirects before the move has started</t>
-  </si>
-  <si>
-    <t>Standard move without prices</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>move not found in JPC</t>
+    <t xml:space="preserve">Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard move</t>
+  </si>
+  <si>
+    <t xml:space="preserve">includes single journeys, cross supplier and redirects before the move has started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard move without prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--</t>
+  </si>
+  <si>
+    <t xml:space="preserve">move not found in JPC</t>
   </si>
   <si>
     <t xml:space="preserve">Long haul </t>
   </si>
   <si>
-    <t>a completed move made up of 2 or more journeys</t>
-  </si>
-  <si>
-    <t>Redirections</t>
-  </si>
-  <si>
-    <t>a redirection after the move has started</t>
-  </si>
-  <si>
-    <t>Lockouts</t>
-  </si>
-  <si>
-    <t>refused admission to prison</t>
-  </si>
-  <si>
-    <t>Multi-type moves</t>
-  </si>
-  <si>
-    <t>includes combinations of the above</t>
-  </si>
-  <si>
-    <t>Total %</t>
-  </si>
-  <si>
-    <t>Total Volume</t>
-  </si>
-  <si>
-    <t>Total Price</t>
+    <t xml:space="preserve">a completed move made up of 2 or more journeys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redirections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a redirection after the move has started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lockouts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refused admission to prison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-type moves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">includes combinations of the above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Price</t>
   </si>
   <si>
     <r>
@@ -137,64 +133,66 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">STANDARD MOVES </t>
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="11"/>
         <rFont val="Cambria"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t>(includes single journeys, cross supplier and redirects before the move has started)</t>
+      <t xml:space="preserve">(includes single journeys, cross supplier and redirects before the move has started)</t>
     </r>
   </si>
   <si>
-    <t>Move Ref ID</t>
-  </si>
-  <si>
-    <t>Pick up</t>
-  </si>
-  <si>
-    <t>Location Type</t>
-  </si>
-  <si>
-    <t>Drop off</t>
-  </si>
-  <si>
-    <t>Pick up date</t>
-  </si>
-  <si>
-    <t>Pick up time</t>
-  </si>
-  <si>
-    <t>Drop off date</t>
-  </si>
-  <si>
-    <t>Drop off time</t>
-  </si>
-  <si>
-    <t>Vehicle Reg No</t>
-  </si>
-  <si>
-    <t>NOMIS Prison ID</t>
-  </si>
-  <si>
-    <t>LONG HAUL</t>
-  </si>
-  <si>
-    <t>Move ID</t>
-  </si>
-  <si>
-    <t>Vehicle ID</t>
-  </si>
-  <si>
-    <t>Contractor Billable?</t>
-  </si>
-  <si>
-    <t>Notes</t>
+    <t xml:space="preserve">Move Ref ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop off date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop off time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle Reg No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOMIS Prison ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LONG HAUL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contractor Billable?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
   </si>
   <si>
     <r>
@@ -202,27 +200,30 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">REDIRECTIONS </t>
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="11"/>
         <rFont val="Cambria"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t>(a redirection after the move has started)</t>
+      <t xml:space="preserve">(a redirection after the move has started)</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
-        <b/>
+        <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Notes </t>
@@ -231,9 +232,10 @@
       <rPr>
         <sz val="11"/>
         <rFont val="Cambria"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t>(Reason codes or supplier notes)</t>
+      <t xml:space="preserve">(Reason codes or supplier notes)</t>
     </r>
   </si>
   <si>
@@ -242,22 +244,24 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">LOCKOUTS </t>
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="9"/>
         <rFont val="Cambria"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t>(refused admission to prison)</t>
+      <t xml:space="preserve">(refused admission to prison)</t>
     </r>
   </si>
   <si>
-    <t>Date range</t>
+    <t xml:space="preserve">Date range</t>
   </si>
   <si>
     <r>
@@ -265,92 +269,123 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t>MULTI-TYPE MOVES</t>
+      <t xml:space="preserve">MULTI-TYPE MOVES</t>
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="11"/>
         <rFont val="Cambria"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> (includes combinations of move types)</t>
     </r>
   </si>
   <si>
-    <t>This needs to be either password protected or interstitial confidentiality agreement per Commercials req</t>
+    <t xml:space="preserve">This needs to be either password protected or interstitial confidentiality agreement per Commercials req</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="\£#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="6">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="0%"/>
+    <numFmt numFmtId="167" formatCode="#,##0"/>
+    <numFmt numFmtId="168" formatCode="\£#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <i val="true"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <i val="true"/>
       <sz val="11"/>
       <name val="Cambria"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <i val="true"/>
       <sz val="9"/>
       <name val="Cambria"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -411,7 +446,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -419,91 +454,197 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="39">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -562,342 +703,36 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
-    <col min="5" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="2" t="n">
         <v>43862</v>
       </c>
       <c r="C1" s="3"/>
@@ -927,7 +762,7 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" spans="1:26" ht="15">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -960,7 +795,7 @@
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
     </row>
-    <row r="3" spans="1:26" ht="14">
+    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -987,7 +822,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26" ht="14">
+    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -1018,7 +853,7 @@
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
     </row>
-    <row r="5" spans="1:26" ht="14">
+    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1049,17 +884,17 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26" ht="14">
+    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="9" t="n">
         <v>43831</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="9" t="n">
         <v>43861</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -1086,7 +921,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:26" ht="14">
+    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1114,7 +949,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26" ht="14">
+    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
@@ -1144,7 +979,7 @@
       <c r="Y8" s="11"/>
       <c r="Z8" s="11"/>
     </row>
-    <row r="9" spans="1:26" ht="14">
+    <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
@@ -1180,17 +1015,17 @@
       <c r="Y9" s="14"/>
       <c r="Z9" s="14"/>
     </row>
-    <row r="10" spans="1:26" ht="14">
+    <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="16" t="n">
         <v>0.9</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="17" t="n">
         <v>9000</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="18" t="n">
         <v>90000</v>
       </c>
       <c r="E10" s="3"/>
@@ -1216,7 +1051,7 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
     </row>
-    <row r="11" spans="1:26" ht="14">
+    <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
         <v>18</v>
       </c>
@@ -1246,7 +1081,7 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" ht="14">
+    <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="20"/>
@@ -1274,14 +1109,14 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26" ht="14">
+    <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="16" t="n">
         <v>0.05</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="17" t="n">
         <v>500</v>
       </c>
       <c r="D13" s="22" t="s">
@@ -1310,7 +1145,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:26" ht="14">
+    <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="s">
         <v>21</v>
       </c>
@@ -1340,7 +1175,7 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:26" ht="14">
+    <row r="15" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1368,14 +1203,14 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:26" ht="14">
+    <row r="16" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="24" t="n">
         <v>0.01</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="15" t="n">
         <v>100</v>
       </c>
       <c r="D16" s="22" t="s">
@@ -1404,7 +1239,7 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:26" ht="14">
+    <row r="17" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19" t="s">
         <v>23</v>
       </c>
@@ -1431,7 +1266,7 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:26" ht="14">
+    <row r="18" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="19"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1459,14 +1294,14 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
     </row>
-    <row r="19" spans="1:26" ht="14">
+    <row r="19" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="16" t="n">
         <v>0.01</v>
       </c>
-      <c r="C19" s="25">
+      <c r="C19" s="25" t="n">
         <v>100</v>
       </c>
       <c r="D19" s="22" t="s">
@@ -1495,7 +1330,7 @@
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
     </row>
-    <row r="20" spans="1:26" ht="14">
+    <row r="20" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="19" t="s">
         <v>25</v>
       </c>
@@ -1525,7 +1360,7 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
     </row>
-    <row r="21" spans="1:26" ht="14">
+    <row r="21" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1553,14 +1388,14 @@
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
     </row>
-    <row r="22" spans="1:26" ht="14">
+    <row r="22" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="16">
+      <c r="B22" s="16" t="n">
         <v>0.01</v>
       </c>
-      <c r="C22" s="25">
+      <c r="C22" s="25" t="n">
         <v>100</v>
       </c>
       <c r="D22" s="22" t="s">
@@ -1589,7 +1424,7 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" ht="14">
+    <row r="23" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="19" t="s">
         <v>27</v>
       </c>
@@ -1619,7 +1454,7 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
     </row>
-    <row r="24" spans="1:26" ht="14">
+    <row r="24" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1647,14 +1482,14 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
     </row>
-    <row r="25" spans="1:26" ht="14">
+    <row r="25" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="16">
+      <c r="B25" s="16" t="n">
         <v>0.02</v>
       </c>
-      <c r="C25" s="25">
+      <c r="C25" s="25" t="n">
         <v>200</v>
       </c>
       <c r="D25" s="22" t="s">
@@ -1683,7 +1518,7 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
     </row>
-    <row r="26" spans="1:26" ht="14">
+    <row r="26" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="19" t="s">
         <v>29</v>
       </c>
@@ -1713,7 +1548,7 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
     </row>
-    <row r="27" spans="1:26" ht="14">
+    <row r="27" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1741,7 +1576,7 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
     </row>
-    <row r="28" spans="1:26" ht="14">
+    <row r="28" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8"/>
       <c r="B28" s="26" t="s">
         <v>30</v>
@@ -1775,12 +1610,12 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
     </row>
-    <row r="29" spans="1:26" ht="14">
+    <row r="29" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3"/>
-      <c r="B29" s="27">
+      <c r="B29" s="27" t="n">
         <v>100</v>
       </c>
-      <c r="C29" s="17">
+      <c r="C29" s="17" t="n">
         <v>10000</v>
       </c>
       <c r="D29" s="22" t="s">
@@ -1809,7 +1644,7 @@
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
     </row>
-    <row r="30" spans="1:26" ht="14">
+    <row r="30" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
       <c r="B30" s="24"/>
       <c r="C30" s="3"/>
@@ -1837,7 +1672,7 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
     </row>
-    <row r="31" spans="1:26" ht="14">
+    <row r="31" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1865,36 +1700,44 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="28"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" customWidth="1"/>
-    <col min="11" max="11" width="18.5" customWidth="1"/>
-    <col min="12" max="1022" width="14.5" customWidth="1"/>
-    <col min="1023" max="1025" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="12" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="14">
+    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1928,7 +1771,7 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="2" spans="1:30" ht="14">
+    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1961,7 +1804,7 @@
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
     </row>
-    <row r="3" spans="1:30" ht="14">
+    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1992,7 +1835,7 @@
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
     </row>
-    <row r="4" spans="1:30" ht="14">
+    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -2026,7 +1869,7 @@
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
     </row>
-    <row r="5" spans="1:30" ht="14">
+    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2060,7 +1903,7 @@
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
     </row>
-    <row r="6" spans="1:30" ht="14">
+    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -2096,7 +1939,7 @@
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
     </row>
-    <row r="7" spans="1:30" ht="14">
+    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2128,7 +1971,7 @@
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
     </row>
-    <row r="8" spans="1:30" ht="14">
+    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>33</v>
       </c>
@@ -2162,7 +2005,7 @@
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
     </row>
-    <row r="9" spans="1:30" ht="12.75" customHeight="1">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
         <v>34</v>
       </c>
@@ -2218,73 +2061,81 @@
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
     </row>
-    <row r="1048540" ht="12.75" customHeight="1"/>
-    <row r="1048541" ht="12.75" customHeight="1"/>
-    <row r="1048542" ht="12.75" customHeight="1"/>
-    <row r="1048543" ht="12.75" customHeight="1"/>
-    <row r="1048544" ht="12.75" customHeight="1"/>
-    <row r="1048545" ht="12.75" customHeight="1"/>
-    <row r="1048546" ht="12.75" customHeight="1"/>
-    <row r="1048547" ht="12.75" customHeight="1"/>
-    <row r="1048548" ht="12.75" customHeight="1"/>
-    <row r="1048549" ht="12.75" customHeight="1"/>
-    <row r="1048550" ht="12.75" customHeight="1"/>
-    <row r="1048551" ht="12.75" customHeight="1"/>
-    <row r="1048552" ht="12.75" customHeight="1"/>
-    <row r="1048553" ht="12.75" customHeight="1"/>
-    <row r="1048554" ht="12.75" customHeight="1"/>
-    <row r="1048555" ht="12.75" customHeight="1"/>
-    <row r="1048556" ht="12.75" customHeight="1"/>
-    <row r="1048557" ht="12.75" customHeight="1"/>
-    <row r="1048558" ht="12.75" customHeight="1"/>
-    <row r="1048559" ht="12.75" customHeight="1"/>
-    <row r="1048560" ht="12.75" customHeight="1"/>
-    <row r="1048561" ht="12.75" customHeight="1"/>
-    <row r="1048562" ht="12.75" customHeight="1"/>
-    <row r="1048563" ht="12.75" customHeight="1"/>
-    <row r="1048564" ht="12.75" customHeight="1"/>
-    <row r="1048565" ht="12.75" customHeight="1"/>
-    <row r="1048566" ht="12.75" customHeight="1"/>
-    <row r="1048567" ht="12.75" customHeight="1"/>
-    <row r="1048568" ht="12.75" customHeight="1"/>
-    <row r="1048569" ht="12.75" customHeight="1"/>
-    <row r="1048570" ht="12.75" customHeight="1"/>
-    <row r="1048571" ht="12.75" customHeight="1"/>
-    <row r="1048572" ht="12.75" customHeight="1"/>
-    <row r="1048573" ht="12.75" customHeight="1"/>
-    <row r="1048574" ht="12.75" customHeight="1"/>
-    <row r="1048575" ht="12.75" customHeight="1"/>
-    <row r="1048576" ht="12.75" customHeight="1"/>
+    <row r="1048540" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="48.5" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" customWidth="1"/>
-    <col min="12" max="12" width="14.5" customWidth="1"/>
-    <col min="13" max="13" width="20.5" customWidth="1"/>
-    <col min="14" max="14" width="24.83203125" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="24.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14">
+    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2302,7 +2153,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:26" ht="14">
+    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2319,7 +2170,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:26" ht="14">
+    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2334,7 +2185,7 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:26" ht="14">
+    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -2352,7 +2203,7 @@
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
     </row>
-    <row r="5" spans="1:26" ht="14">
+    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2370,7 +2221,7 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:26" ht="14">
+    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -2390,7 +2241,7 @@
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:26" ht="14">
+    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2406,7 +2257,7 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:26" ht="14">
+    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
@@ -2424,7 +2275,7 @@
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
     </row>
-    <row r="9" spans="1:26" ht="30">
+    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
         <v>45</v>
       </c>
@@ -2480,39 +2331,47 @@
       <c r="Y9" s="34"/>
       <c r="Z9" s="34"/>
     </row>
-    <row r="1048561" ht="15.75" customHeight="1"/>
-    <row r="1048562" ht="12.75" customHeight="1"/>
-    <row r="1048576" ht="12.75" customHeight="1"/>
+    <row r="1048561" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD1048576"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="52" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="18.5" customWidth="1"/>
-    <col min="12" max="12" width="9.1640625" customWidth="1"/>
-    <col min="13" max="13" width="20.1640625" customWidth="1"/>
-    <col min="14" max="14" width="32.5" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="32.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="14">
+    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2546,7 +2405,7 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="2" spans="1:30" ht="14">
+    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2579,7 +2438,7 @@
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
     </row>
-    <row r="3" spans="1:30" ht="14">
+    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2610,7 +2469,7 @@
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
     </row>
-    <row r="4" spans="1:30" ht="14">
+    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -2644,7 +2503,7 @@
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
     </row>
-    <row r="5" spans="1:30" ht="14">
+    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2678,7 +2537,7 @@
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
     </row>
-    <row r="6" spans="1:30" ht="14">
+    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -2714,7 +2573,7 @@
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
     </row>
-    <row r="7" spans="1:30" ht="14">
+    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2746,7 +2605,7 @@
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
     </row>
-    <row r="8" spans="1:30" ht="14">
+    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>49</v>
       </c>
@@ -2780,7 +2639,7 @@
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
     </row>
-    <row r="9" spans="1:30" ht="45">
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
         <v>45</v>
       </c>
@@ -2840,48 +2699,56 @@
       <c r="AC9" s="15"/>
       <c r="AD9" s="15"/>
     </row>
-    <row r="1048562" ht="12.75" customHeight="1"/>
-    <row r="1048563" ht="12.75" customHeight="1"/>
-    <row r="1048564" ht="12.75" customHeight="1"/>
-    <row r="1048565" ht="12.75" customHeight="1"/>
-    <row r="1048566" ht="12.75" customHeight="1"/>
-    <row r="1048567" ht="12.75" customHeight="1"/>
-    <row r="1048568" ht="12.75" customHeight="1"/>
-    <row r="1048569" ht="12.75" customHeight="1"/>
-    <row r="1048570" ht="12.75" customHeight="1"/>
-    <row r="1048571" ht="12.75" customHeight="1"/>
-    <row r="1048572" ht="12.75" customHeight="1"/>
-    <row r="1048573" ht="12.75" customHeight="1"/>
-    <row r="1048574" ht="12.75" customHeight="1"/>
-    <row r="1048575" ht="12.75" customHeight="1"/>
-    <row r="1048576" ht="12.75" customHeight="1"/>
+    <row r="1048562" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AF1048576"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="7.1640625" customWidth="1"/>
-    <col min="4" max="4" width="28.5" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" customWidth="1"/>
-    <col min="6" max="13" width="14.5" customWidth="1"/>
-    <col min="14" max="14" width="31.33203125" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="31.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="14">
+    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2917,7 +2784,7 @@
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
     </row>
-    <row r="2" spans="1:32" ht="14">
+    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2952,7 +2819,7 @@
       <c r="AE2" s="3"/>
       <c r="AF2" s="3"/>
     </row>
-    <row r="3" spans="1:32" ht="14">
+    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2985,7 +2852,7 @@
       <c r="AE3" s="3"/>
       <c r="AF3" s="3"/>
     </row>
-    <row r="4" spans="1:32" ht="14">
+    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -3021,7 +2888,7 @@
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
     </row>
-    <row r="5" spans="1:32" ht="14">
+    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -3057,7 +2924,7 @@
       <c r="AE5" s="3"/>
       <c r="AF5" s="3"/>
     </row>
-    <row r="6" spans="1:32" ht="14">
+    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -3095,7 +2962,7 @@
       <c r="AE6" s="3"/>
       <c r="AF6" s="3"/>
     </row>
-    <row r="7" spans="1:32" ht="14">
+    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -3129,7 +2996,7 @@
       <c r="AE7" s="3"/>
       <c r="AF7" s="3"/>
     </row>
-    <row r="8" spans="1:32" ht="14">
+    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>51</v>
       </c>
@@ -3165,7 +3032,7 @@
       <c r="AE8" s="3"/>
       <c r="AF8" s="3"/>
     </row>
-    <row r="9" spans="1:32" ht="45">
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
         <v>34</v>
       </c>
@@ -3227,57 +3094,65 @@
       <c r="AE9" s="3"/>
       <c r="AF9" s="3"/>
     </row>
-    <row r="1048559" ht="12.75" customHeight="1"/>
-    <row r="1048560" ht="12.75" customHeight="1"/>
-    <row r="1048561" ht="12.75" customHeight="1"/>
-    <row r="1048562" ht="12.75" customHeight="1"/>
-    <row r="1048563" ht="12.75" customHeight="1"/>
-    <row r="1048564" ht="12.75" customHeight="1"/>
-    <row r="1048565" ht="12.75" customHeight="1"/>
-    <row r="1048566" ht="12.75" customHeight="1"/>
-    <row r="1048567" ht="12.75" customHeight="1"/>
-    <row r="1048568" ht="12.75" customHeight="1"/>
-    <row r="1048569" ht="12.75" customHeight="1"/>
-    <row r="1048570" ht="12.75" customHeight="1"/>
-    <row r="1048571" ht="12.75" customHeight="1"/>
-    <row r="1048572" ht="12.75" customHeight="1"/>
-    <row r="1048573" ht="12.75" customHeight="1"/>
-    <row r="1048574" ht="12.75" customHeight="1"/>
-    <row r="1048575" ht="12.75" customHeight="1"/>
-    <row r="1048576" ht="12.75" customHeight="1"/>
+    <row r="1048559" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L24" activeCellId="0" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="66.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.1640625" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.5" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" customWidth="1"/>
-    <col min="9" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" customWidth="1"/>
-    <col min="13" max="13" width="10.1640625" customWidth="1"/>
-    <col min="14" max="14" width="30" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="30.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="14">
+    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3311,7 +3186,7 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="2" spans="1:30" ht="14">
+    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3344,7 +3219,7 @@
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
     </row>
-    <row r="3" spans="1:30" ht="14">
+    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -3375,7 +3250,7 @@
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
     </row>
-    <row r="4" spans="1:30" ht="14">
+    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -3409,7 +3284,7 @@
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
     </row>
-    <row r="5" spans="1:30" ht="14">
+    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -3443,7 +3318,7 @@
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
     </row>
-    <row r="6" spans="1:30" ht="14">
+    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -3479,7 +3354,7 @@
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
     </row>
-    <row r="7" spans="1:30" ht="14">
+    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -3511,7 +3386,7 @@
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
     </row>
-    <row r="8" spans="1:30" ht="14">
+    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>53</v>
       </c>
@@ -3545,7 +3420,7 @@
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
     </row>
-    <row r="9" spans="1:30" ht="30">
+    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
         <v>45</v>
       </c>
@@ -3605,49 +3480,90 @@
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
     </row>
-    <row r="1048559" ht="12.75" customHeight="1"/>
-    <row r="1048560" ht="12.75" customHeight="1"/>
-    <row r="1048561" ht="12.75" customHeight="1"/>
-    <row r="1048562" ht="12.75" customHeight="1"/>
-    <row r="1048563" ht="12.75" customHeight="1"/>
-    <row r="1048564" ht="12.75" customHeight="1"/>
-    <row r="1048565" ht="12.75" customHeight="1"/>
-    <row r="1048566" ht="12.75" customHeight="1"/>
-    <row r="1048567" ht="12.75" customHeight="1"/>
-    <row r="1048568" ht="12.75" customHeight="1"/>
-    <row r="1048569" ht="12.75" customHeight="1"/>
-    <row r="1048570" ht="12.75" customHeight="1"/>
-    <row r="1048571" ht="12.75" customHeight="1"/>
-    <row r="1048572" ht="12.75" customHeight="1"/>
-    <row r="1048573" ht="12.75" customHeight="1"/>
-    <row r="1048574" ht="12.75" customHeight="1"/>
-    <row r="1048575" ht="12.75" customHeight="1"/>
-    <row r="1048576" ht="12.75" customHeight="1"/>
+    <row r="1048559" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="43" customWidth="1"/>
-    <col min="2" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="45">
+    <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>